<commit_message>
cleanup prior to python 3 test;  possibly broken due to library breakage
</commit_message>
<xml_diff>
--- a/tests/modelAnswer.xlsx
+++ b/tests/modelAnswer.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="122">
   <si>
     <t>I25.11</t>
   </si>
@@ -742,12 +742,12 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B14"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.140625" bestFit="1" customWidth="1"/>
@@ -759,10 +759,10 @@
         <v>118</v>
       </c>
       <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
         <v>120</v>
-      </c>
-      <c r="C1" t="s">
-        <v>117</v>
       </c>
       <c r="D1" t="s">
         <v>104</v>
@@ -779,10 +779,10 @@
         <v>116</v>
       </c>
       <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>121</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>116</v>
@@ -793,10 +793,10 @@
         <v>116</v>
       </c>
       <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>121</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,10 +804,16 @@
         <v>116</v>
       </c>
       <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>121</v>
       </c>
-      <c r="C4" t="s">
-        <v>2</v>
+      <c r="D4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -815,10 +821,13 @@
         <v>116</v>
       </c>
       <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
         <v>121</v>
       </c>
-      <c r="C5" t="s">
-        <v>3</v>
+      <c r="D5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,16 +835,19 @@
         <v>116</v>
       </c>
       <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
         <v>121</v>
       </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
       <c r="D6" t="s">
         <v>108</v>
       </c>
       <c r="E6">
         <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -843,10 +855,10 @@
         <v>116</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
       </c>
       <c r="D7" t="s">
         <v>108</v>
@@ -860,10 +872,10 @@
         <v>116</v>
       </c>
       <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>108</v>
@@ -877,10 +889,10 @@
         <v>116</v>
       </c>
       <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>108</v>
@@ -894,10 +906,10 @@
         <v>116</v>
       </c>
       <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
         <v>121</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -905,10 +917,10 @@
         <v>116</v>
       </c>
       <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -916,10 +928,10 @@
         <v>116</v>
       </c>
       <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,10 +939,13 @@
         <v>116</v>
       </c>
       <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
         <v>121</v>
       </c>
-      <c r="C13" t="s">
-        <v>11</v>
+      <c r="D13" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -938,10 +953,13 @@
         <v>116</v>
       </c>
       <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
         <v>121</v>
       </c>
-      <c r="C14" t="s">
-        <v>12</v>
+      <c r="D14" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>